<commit_message>
Backup: Before Revise contrastive decoding-v2temp
</commit_message>
<xml_diff>
--- a/eval_results_pid.xlsx
+++ b/eval_results_pid.xlsx
@@ -487,22 +487,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="D2" t="n">
-        <v>0.035</v>
+        <v>0.037</v>
       </c>
       <c r="E2" t="n">
-        <v>0.049</v>
+        <v>0.053</v>
       </c>
       <c r="F2" t="n">
-        <v>0.079</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>0.106</v>
+        <v>0.114</v>
       </c>
       <c r="H2" t="n">
-        <v>0.146</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="3">
@@ -517,22 +517,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.001763492063492064</v>
+        <v>0.002285714285714286</v>
       </c>
       <c r="D3" t="n">
-        <v>0.005897619047619049</v>
+        <v>0.006253174603174603</v>
       </c>
       <c r="E3" t="n">
-        <v>0.009034920634920634</v>
+        <v>0.01024761904761904</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01402142857142856</v>
+        <v>0.01538412698412697</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02144365079365078</v>
+        <v>0.02327420634920634</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03048412698412697</v>
+        <v>0.03309246031746031</v>
       </c>
     </row>
     <row r="4">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01259216382193173</v>
+        <v>0.01353072127397724</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01221260054110822</v>
+        <v>0.01317972828356509</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01269416907414274</v>
+        <v>0.01374058675776681</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01573423036293674</v>
+        <v>0.01700362346505621</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01917535472884331</v>
+        <v>0.02068832803497481</v>
       </c>
     </row>
     <row r="5">
@@ -580,10 +580,10 @@
         <v>0.02</v>
       </c>
       <c r="D5" t="n">
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
       <c r="E5" t="n">
-        <v>0.067</v>
+        <v>0.068</v>
       </c>
       <c r="F5" t="n">
         <v>0.1</v>
@@ -610,19 +610,19 @@
         <v>0.002411111111111111</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006695238095238093</v>
+        <v>0.006795238095238092</v>
       </c>
       <c r="E6" t="n">
-        <v>0.009074999999999995</v>
+        <v>0.009174999999999994</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01504920634920633</v>
+        <v>0.01514920634920633</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01744761904761903</v>
+        <v>0.01754761904761903</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02179325396825395</v>
+        <v>0.02189325396825395</v>
       </c>
     </row>
     <row r="7">
@@ -640,19 +640,19 @@
         <v>0.02</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0185699021643186</v>
+        <v>0.01880454152732997</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01628950568083011</v>
+        <v>0.01645908578346691</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01558070180100097</v>
+        <v>0.01569074768415001</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01690077614621596</v>
+        <v>0.01701082202936499</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01895363421332586</v>
+        <v>0.0190636800964749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup: Before Revise contrastive decoding-v3temp
</commit_message>
<xml_diff>
--- a/eval_results_pid.xlsx
+++ b/eval_results_pid.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>ad</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -487,28 +487,28 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.015</v>
+        <v>0.021</v>
       </c>
       <c r="D2" t="n">
-        <v>0.037</v>
+        <v>0.056</v>
       </c>
       <c r="E2" t="n">
-        <v>0.053</v>
+        <v>0.079</v>
       </c>
       <c r="F2" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.109</v>
       </c>
       <c r="G2" t="n">
-        <v>0.114</v>
+        <v>0.156</v>
       </c>
       <c r="H2" t="n">
-        <v>0.155</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>ad</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -517,28 +517,28 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.002285714285714286</v>
+        <v>0.006613492063492063</v>
       </c>
       <c r="D3" t="n">
-        <v>0.006253174603174603</v>
+        <v>0.01824642857142857</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01024761904761904</v>
+        <v>0.02749603174603174</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01538412698412697</v>
+        <v>0.03750039682539683</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02327420634920634</v>
+        <v>0.05507500000000005</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03309246031746031</v>
+        <v>0.07451111111111113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>ad</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -547,28 +547,28 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.015</v>
+        <v>0.021</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01353072127397724</v>
+        <v>0.02254369849090224</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01317972828356509</v>
+        <v>0.02471010461444407</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01374058675776681</v>
+        <v>0.02745757381377225</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01700362346505621</v>
+        <v>0.03377001744513262</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02068832803497481</v>
+        <v>0.04010448322283051</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>product</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -577,28 +577,28 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.02</v>
+        <v>0.012</v>
       </c>
       <c r="D5" t="n">
-        <v>0.052</v>
+        <v>0.037</v>
       </c>
       <c r="E5" t="n">
-        <v>0.068</v>
+        <v>0.054</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1</v>
+        <v>0.083</v>
       </c>
       <c r="G5" t="n">
-        <v>0.115</v>
+        <v>0.114</v>
       </c>
       <c r="H5" t="n">
-        <v>0.146</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>product</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -607,51 +607,141 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.002411111111111111</v>
+        <v>0.001819047619047619</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006795238095238092</v>
+        <v>0.006647619047619048</v>
       </c>
       <c r="E6" t="n">
-        <v>0.009174999999999994</v>
+        <v>0.01078492063492063</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01514920634920633</v>
+        <v>0.01550476190476189</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01754761904761903</v>
+        <v>0.02309642857142856</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02189325396825395</v>
+        <v>0.03220357142857141</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>pid_ndcg</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.01302162251422344</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.01309264166566387</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.01345816976840837</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.01659217718367545</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.02002961693412586</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>video</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>pid_pass</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.146</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>pid_recall</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.002411111111111111</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.006795238095238092</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.009174999999999994</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.01514920634920633</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.01754761904761903</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.02189325396825395</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>pid_ndcg</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C10" t="n">
         <v>0.02</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D10" t="n">
         <v>0.01880454152732997</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E10" t="n">
         <v>0.01645908578346691</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F10" t="n">
         <v>0.01569074768415001</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G10" t="n">
         <v>0.01701082202936499</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H10" t="n">
         <v>0.0190636800964749</v>
       </c>
     </row>

</xml_diff>